<commit_message>
CHANGED: Entire team -> ONE person of the team as responsible person in risk analysis
</commit_message>
<xml_diff>
--- a/SoftwareEngeneering/RiskAnalysis.xlsx
+++ b/SoftwareEngeneering/RiskAnalysis.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpenkert/Development/SimpleHabits/SoftwareEngeneering/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bene/Documents/Programmieren/SimpleHabits/SoftwareEngeneering/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Risk Managment</t>
   </si>
@@ -92,10 +92,13 @@
     <t>--</t>
   </si>
   <si>
-    <t>entire team</t>
-  </si>
-  <si>
     <t>Deadline Pressure</t>
+  </si>
+  <si>
+    <t>René Penkert</t>
+  </si>
+  <si>
+    <t>Benedikt Bosshammer</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
   <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,12 +491,12 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="48" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -505,14 +508,14 @@
         <v>3</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F5:F10" si="0">E6*D6</f>
+        <f t="shared" ref="F6:F10" si="0">E6*D6</f>
         <v>1.7999999999999998</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="48" x14ac:dyDescent="0.2">
@@ -536,7 +539,7 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="80" x14ac:dyDescent="0.2">
@@ -560,7 +563,7 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="32" x14ac:dyDescent="0.2">
@@ -582,7 +585,7 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
@@ -602,7 +605,7 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Risk Analysis print format
</commit_message>
<xml_diff>
--- a/SoftwareEngeneering/RiskAnalysis.xlsx
+++ b/SoftwareEngeneering/RiskAnalysis.xlsx
@@ -5,15 +5,20 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpenkert/Development/AlarmClock/SimpleHabits/SoftwareEngeneering/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bene/Documents/Programmieren/SimpleHabits/SoftwareEngeneering/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$B$1:$H$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Tabelle2!$B$2:$P$24</definedName>
+  </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -29,9 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
-    <t>Risk Managment</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -41,12 +43,6 @@
     <t>Propability</t>
   </si>
   <si>
-    <t>Impact</t>
-  </si>
-  <si>
-    <t>1 not much impact. 10 huge impact</t>
-  </si>
-  <si>
     <t>Factor</t>
   </si>
   <si>
@@ -132,6 +128,15 @@
   </si>
   <si>
     <t>Decreased SE Risk because we are right on schedule for the final SE exam</t>
+  </si>
+  <si>
+    <t>*1 not much impact. 10 huge impact</t>
+  </si>
+  <si>
+    <t>Impact*</t>
+  </si>
+  <si>
+    <t>Risk Management</t>
   </si>
 </sst>
 </file>
@@ -147,14 +152,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="24"/>
-      <color rgb="FFFF0000"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -201,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -230,7 +237,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -508,75 +519,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I20"/>
+  <dimension ref="B2:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.83203125" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="M3" s="12"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="2:9" ht="80" x14ac:dyDescent="0.2">
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="2:13" ht="96" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" s="7">
         <v>0.6</v>
@@ -589,19 +601,19 @@
         <v>4.2</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="2:9" ht="48" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="2:13" ht="48" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D6" s="7">
         <v>0.6</v>
@@ -614,19 +626,19 @@
         <v>1.7999999999999998</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="2:9" ht="48" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="2:13" ht="64" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7" s="7">
         <v>0.4</v>
@@ -639,19 +651,19 @@
         <v>1.6</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="2:9" ht="80" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="2:13" ht="112" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" s="7">
         <v>0.8</v>
@@ -664,19 +676,19 @@
         <v>0.8</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="2:9" ht="32" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="2:13" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D9" s="7">
         <v>0.05</v>
@@ -689,16 +701,16 @@
         <v>0.4</v>
       </c>
       <c r="G9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="7">
@@ -712,168 +724,145 @@
         <v>0.2</v>
       </c>
       <c r="G10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="2:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="B12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="5"/>
-      <c r="C13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="2">
-        <v>42852</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="5"/>
-      <c r="C14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="2">
-        <v>42854</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="5"/>
-      <c r="C15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="2">
-        <v>42862</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B16" s="5"/>
-      <c r="C16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="2">
-        <v>42865</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-      <c r="C17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="2">
-        <v>42870</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
-      <c r="C18" s="4" t="s">
+      <c r="I10" s="12"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="2">
-        <v>42880</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B19" s="5"/>
-      <c r="C19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="2">
-        <v>42891</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B20" s="5"/>
-      <c r="C20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="2">
-        <v>42902</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
     </row>
   </sheetData>
   <sortState ref="B5:H10">
     <sortCondition descending="1" ref="F5:F10"/>
   </sortState>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="N3:P12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="65" customWidth="1"/>
+    <col min="15" max="15" width="26.33203125" customWidth="1"/>
+    <col min="16" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="14:16" x14ac:dyDescent="0.2">
+      <c r="N3" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="14:16" x14ac:dyDescent="0.2">
+      <c r="N4" s="13"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+    </row>
+    <row r="5" spans="14:16" x14ac:dyDescent="0.2">
+      <c r="N5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="2">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="6" spans="14:16" x14ac:dyDescent="0.2">
+      <c r="N6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="2">
+        <v>42854</v>
+      </c>
+    </row>
+    <row r="7" spans="14:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="2">
+        <v>42862</v>
+      </c>
+    </row>
+    <row r="8" spans="14:16" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8" s="2">
+        <v>42865</v>
+      </c>
+    </row>
+    <row r="9" spans="14:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="2">
+        <v>42870</v>
+      </c>
+    </row>
+    <row r="10" spans="14:16" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="2">
+        <v>42880</v>
+      </c>
+    </row>
+    <row r="11" spans="14:16" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" s="2">
+        <v>42891</v>
+      </c>
+    </row>
+    <row r="12" spans="14:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P12" s="2">
+        <v>42902</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>